<commit_message>
update A1-A20 STAGE-1 STAGE-2
</commit_message>
<xml_diff>
--- a/SandraGarc/evidence.xlsx
+++ b/SandraGarc/evidence.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>TxHash</t>
   </si>
@@ -57,27 +57,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -172,6 +157,159 @@
   </si>
   <si>
     <t>BA389200A3FF0E93F6892A2494DF58C678BCA3794886EC6C9E2841C6FBD7DBCB</t>
+  </si>
+  <si>
+    <t>ibc/422A1610884E7B29CADB4F1D1287B4859A6D962CF705BECD0CB0793F85596111</t>
+  </si>
+  <si>
+    <t>syndicate7</t>
+  </si>
+  <si>
+    <t>ibc/EBB35299A0D19CC0EC25B10E042D3F67D47CA10BA215A7C02339B172FA633DBB</t>
+  </si>
+  <si>
+    <t>syndicate8</t>
+  </si>
+  <si>
+    <t>ibc/67A7C0635612A89C4F62777F70D5F742883712177506E7528152CD1AD4CB10B7</t>
+  </si>
+  <si>
+    <t>syndicate9</t>
+  </si>
+  <si>
+    <t>ibc/206330D6F2DA67DB279A12569850D5EE7168E13886D36AA233B6267F3044A18A</t>
+  </si>
+  <si>
+    <t>syndicate10</t>
+  </si>
+  <si>
+    <t>ibc/26CC99BB8089A932250F123B53E9CE0A4F2148AD3449554584ACDAEA5496CC3C</t>
+  </si>
+  <si>
+    <t>syndicate11</t>
+  </si>
+  <si>
+    <t>ibc/3507208EE2A41714CBC38A9E52E21BC99C40782E5991F3135E950FB644C325F0</t>
+  </si>
+  <si>
+    <t>syndicate12</t>
+  </si>
+  <si>
+    <t>E55D38B0811EB3EC1887FC82EF45F9575375A4E0C2B67DE0A4EADD229A94F074</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>8A3C2794D0CA7DC8314C63433962AC50AC887A0B91E1533629DFEECA35AB4519</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>B2A0C3C978ED3F027A9D43FCE1190C5384122791E3AAE50E0E389AEE99D849CA</t>
+  </si>
+  <si>
+    <t>8428D86284FEFF9C6985C37ECF66A6666EB280481D376645D104AFFDF1260EA0</t>
+  </si>
+  <si>
+    <t>C5CB019F2FC73E33DC9AB1023BDE089EDF91FBC0DD37AD717EC95DDF86C54895</t>
+  </si>
+  <si>
+    <t>E8E0B1804883C8D0823778DF35CFBA3EB7F7BA2D757F341D1C6C220CFB35D3BB</t>
+  </si>
+  <si>
+    <t>4B30C70633C22A60A7D62C5C57A4099C2EF4F4A674DD348CDBDD9A90E6628487</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>5F55522AB5D2194D8E65962D8D01B1B66F7D455DF1E84854B793320E917AC0EC</t>
+  </si>
+  <si>
+    <t>AF4EBB017CE3D679CEA085A44197CCF2A529CFA1D4E9D9F4E7205248D70BEB33</t>
+  </si>
+  <si>
+    <t>91AF5B8E0368B8D3B889193A460FBECF47072D67E765FADAB9608A56039FED61</t>
+  </si>
+  <si>
+    <t>D62D233C69AAD97A10C41CA54E6856A974B6DEFD598078F607A03EC96A181B8D</t>
+  </si>
+  <si>
+    <t>7075EB31E19356F8F7CB69496B2C28A0D06F11223EFE64C3145A0F11491951E4</t>
+  </si>
+  <si>
+    <t>CBB99C180B3BA94DC90DA17E4D40DF6CCDD2A298712F30A70EF7DA2E47B3C7B1</t>
+  </si>
+  <si>
+    <t>994017F17DE5A5BABE32A1B0B8B24207C9209C7D99CE24E3EFD02C8CFFFD5CF9</t>
+  </si>
+  <si>
+    <t>53BF4E61B1602A16E426A66753F04B5327D1386DC44AFF7E4343979138724ACA</t>
+  </si>
+  <si>
+    <t>F1EEA948DDA5AE57C1E3F69AEFDB846FE724BB6831F87CDAA12EE6FC3C08DE0B</t>
+  </si>
+  <si>
+    <t>31046133628EA868D241BB33D0AE942439A70B3CCE89FD6BA33B781F3DEEA3AD</t>
+  </si>
+  <si>
+    <t>1B7D9FA311BA44431F3BB6F799C098CAABDAF584BCFA785890DACC67CD992ABE</t>
+  </si>
+  <si>
+    <t>BDF3F39615C894C0480C6741BA2DF9ABE8176C90188623B575A5A728EBBBD5AA</t>
+  </si>
+  <si>
+    <t>B6D9B26C5C4F56A6B224D86ACC366C53D1571724F6665ED25533DEE0A53F9CC6</t>
+  </si>
+  <si>
+    <t>B0E2E2159C6D435F384EBD4B127D6DB607A4886B82D9DE497B91FADDDAAA7833</t>
+  </si>
+  <si>
+    <t>787B348C04C420F07D591B36FDC39B6CC35E34DFE40FF657E59116EC738ED467</t>
+  </si>
+  <si>
+    <t>40910C5E631EC20EFC03C1E95E8660CCD276A99A57457B2A0291A6685E23037B</t>
+  </si>
+  <si>
+    <t>08A572BD128D89957CD5640BB0FE4CDFA54A989F41F8D77A142B07F7C104BEDA</t>
+  </si>
+  <si>
+    <t>F9020B9971714495C8757838A185D8EC682AA5FF7DD5E41C6C4CD7202C6E584F</t>
+  </si>
+  <si>
+    <t>2AB1269F7FF176996549159B8AADB80616322D7BD0B0DCAE670F103032719313</t>
+  </si>
+  <si>
+    <t>BF14FB2687057173432D0CBB15A1D30AFDCA2A1E47FDE7C313AAD86D5F423EA5</t>
+  </si>
+  <si>
+    <t>3EAAE51B00997BD60C7CE082A22B536815069D0A0B4943F155C830DBFAC6DFCA</t>
+  </si>
+  <si>
+    <t>415A897B3BBDA9730756822780CBEC842861D06343CCB9E439DF390D4C40FFAC</t>
+  </si>
+  <si>
+    <t>87D72F04886990E65306ED90C67CCB720B0C96FB2AE363485CFF89F81A68D430</t>
+  </si>
+  <si>
+    <t>13CFA90A6584AFC28BA86FE26FBD357439F22DE1DB27A4D9B3E5590739315DBE</t>
+  </si>
+  <si>
+    <t>F6BE585F0C7F27B1BB12CBEF0B535301617A55FECB74C13014434B9E086E061A</t>
+  </si>
+  <si>
+    <t>4255016E29DA4133AFFF92D637455D6FAB1F8B358B654C8FD6C3C3F03E08ABE0</t>
+  </si>
+  <si>
+    <t>26449700945186D0A42DB9532BABA68ABF930193BFA2EA430BBA612AC737BE1B</t>
+  </si>
+  <si>
+    <t>7AAC07B7AE812A879011148B236B5852FE270F18683CAFFC73039287DB59EC23</t>
+  </si>
+  <si>
+    <t>9767E07DCD45B78D46A952779213DADAF9624A3F49E63391206F6E2E36545F1F</t>
   </si>
 </sst>
 </file>
@@ -586,55 +724,55 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -649,7 +787,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -659,18 +799,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -685,7 +825,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -695,18 +837,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +863,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -731,18 +875,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +901,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -767,18 +913,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -791,9 +937,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -811,23 +959,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -839,9 +999,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -859,23 +1021,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -887,9 +1061,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -907,23 +1083,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -935,9 +1123,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -955,23 +1145,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -983,9 +1185,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1003,23 +1207,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1031,9 +1247,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1051,23 +1269,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1095,15 +1325,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1116,9 +1346,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1136,23 +1368,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1164,9 +1424,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1184,23 +1446,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1365,43 +1655,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1432,10 +1722,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1443,16 +1733,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1483,10 +1773,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1494,16 +1784,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1534,10 +1824,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1545,16 +1835,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1586,10 +1876,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1597,31 +1887,72 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1631,54 +1962,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>